<commit_message>
testing timing of indol 3exp with constraints
</commit_message>
<xml_diff>
--- a/configFiles/2020-03-10_TimingTests.xlsx
+++ b/configFiles/2020-03-10_TimingTests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JLD\GitRepos\flim_flam\configFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D9CBD1-9CE4-4D84-88E2-FC96D7C740E5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A1C6E57-70CF-4616-A460-E9EDF8120F68}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C7F892D4-BF5F-41EB-9A3C-6208354A545F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>maxFunEval</t>
   </si>
@@ -73,13 +73,40 @@
   </si>
   <si>
     <t>lifetime stdev</t>
+  </si>
+  <si>
+    <t>fit results (ns)</t>
+  </si>
+  <si>
+    <t>trial</t>
+  </si>
+  <si>
+    <t>inputs</t>
+  </si>
+  <si>
+    <t>probably still OK but maybe getting borderline?</t>
+  </si>
+  <si>
+    <t>no-brainer to add in this improvement</t>
+  </si>
+  <si>
+    <t>(constraint tol is really just about how close program can get to constraints)</t>
+  </si>
+  <si>
+    <t>(this update sacrifices nothing in accuracy)</t>
+  </si>
+  <si>
+    <t>probably still fine for a faster mode</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,13 +122,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -116,12 +164,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,50 +492,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC10102-7D9D-45CC-8D7B-C4FFE6CCE50F}">
-  <dimension ref="A14:M18"/>
+  <dimension ref="A14:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="12.77734375" customWidth="1"/>
-    <col min="9" max="9" width="14.88671875" customWidth="1"/>
-    <col min="11" max="11" width="15.44140625" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" customWidth="1"/>
+    <col min="9" max="9" width="12.77734375" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="12" max="12" width="15.44140625" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G16" t="s">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B16" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="G16" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="K16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
         <v>0</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>1</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>2</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>3</v>
-      </c>
-      <c r="E17" t="s">
-        <v>5</v>
       </c>
       <c r="G17" t="s">
         <v>7</v>
@@ -491,26 +560,32 @@
         <v>10</v>
       </c>
       <c r="K17" t="s">
+        <v>5</v>
+      </c>
+      <c r="L17" t="s">
         <v>6</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>13</v>
       </c>
-      <c r="M17" s="3" t="s">
+      <c r="N17" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18" s="1">
         <v>100000</v>
       </c>
-      <c r="B18" s="1">
-        <v>1E-4</v>
-      </c>
       <c r="C18" s="1">
         <v>1E-4</v>
       </c>
       <c r="D18" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="E18" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="G18" s="2">
@@ -522,8 +597,307 @@
       <c r="I18" s="2">
         <v>2.6</v>
       </c>
+      <c r="K18" s="5">
+        <v>1.1288</v>
+      </c>
+      <c r="L18" s="5">
+        <v>0.27350000000000002</v>
+      </c>
+      <c r="M18" s="5">
+        <v>3.3300000000000003E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" s="1">
+        <v>100000</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="D19" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="E19" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="H19">
+        <v>79.3</v>
+      </c>
+      <c r="K19">
+        <v>1.1324000000000001</v>
+      </c>
+      <c r="L19">
+        <v>0.2742</v>
+      </c>
+      <c r="M19">
+        <v>3.3500000000000002E-2</v>
+      </c>
+      <c r="O19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20" s="1">
+        <v>100000</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="D20" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E20" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="H20">
+        <v>56.7</v>
+      </c>
+      <c r="K20">
+        <v>1.1591</v>
+      </c>
+      <c r="L20">
+        <v>0.28289999999999998</v>
+      </c>
+      <c r="M20">
+        <v>3.3799999999999997E-2</v>
+      </c>
+      <c r="O20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21" s="1">
+        <v>100000</v>
+      </c>
+      <c r="C21" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="E21" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="H21">
+        <v>48.2</v>
+      </c>
+      <c r="K21" s="9">
+        <v>1.3174999999999999</v>
+      </c>
+      <c r="L21">
+        <v>0.28010000000000002</v>
+      </c>
+      <c r="M21">
+        <v>3.5299999999999998E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>4</v>
+      </c>
+      <c r="B22" s="1">
+        <v>100000</v>
+      </c>
+      <c r="C22" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="E22" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="H22">
+        <v>75.7</v>
+      </c>
+      <c r="K22">
+        <v>1.1956</v>
+      </c>
+      <c r="L22">
+        <v>0.27439999999999998</v>
+      </c>
+      <c r="M22">
+        <v>0.33</v>
+      </c>
+      <c r="O22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23" s="1">
+        <v>100000</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="E23" s="8">
+        <v>1E-4</v>
+      </c>
+      <c r="H23">
+        <v>86.7</v>
+      </c>
+      <c r="K23">
+        <v>1.1288</v>
+      </c>
+      <c r="L23">
+        <v>0.27350000000000002</v>
+      </c>
+      <c r="M23">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="O23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>6</v>
+      </c>
+      <c r="B24" s="1">
+        <v>100000</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="E24" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="H24">
+        <v>86.7</v>
+      </c>
+      <c r="K24">
+        <v>1.1288</v>
+      </c>
+      <c r="L24">
+        <v>0.27350000000000002</v>
+      </c>
+      <c r="M24">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="O24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>7</v>
+      </c>
+      <c r="B25" s="1">
+        <v>100000</v>
+      </c>
+      <c r="C25" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="D25" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="E25" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="H25">
+        <v>70</v>
+      </c>
+      <c r="K25">
+        <v>1.1992</v>
+      </c>
+      <c r="L25">
+        <v>0.27479999999999999</v>
+      </c>
+      <c r="M25">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="O25" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>8</v>
+      </c>
+      <c r="B26" s="1">
+        <v>100000</v>
+      </c>
+      <c r="C26" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="D26" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="E26" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="H26">
+        <v>48</v>
+      </c>
+      <c r="K26">
+        <v>1.3174999999999999</v>
+      </c>
+      <c r="L26">
+        <v>0.28010000000000002</v>
+      </c>
+      <c r="M26">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="O26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>9</v>
+      </c>
+      <c r="B27" s="1">
+        <v>100000</v>
+      </c>
+      <c r="C27" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="D27" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E27" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="H27">
+        <v>45.2</v>
+      </c>
+      <c r="K27">
+        <v>1.3289</v>
+      </c>
+      <c r="L27">
+        <v>0.2833</v>
+      </c>
+      <c r="M27">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="O27" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="K16:M16"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
testing 2exp timing, minor bug fixes
</commit_message>
<xml_diff>
--- a/configFiles/2020-03-10_TimingTests.xlsx
+++ b/configFiles/2020-03-10_TimingTests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JLD\GitRepos\flim_flam\configFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A1C6E57-70CF-4616-A460-E9EDF8120F68}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B892EF8-9C62-4693-A619-F80F59FD950B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C7F892D4-BF5F-41EB-9A3C-6208354A545F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
   <si>
     <t>maxFunEval</t>
   </si>
@@ -45,27 +45,15 @@
     <t>constraintTol</t>
   </si>
   <si>
-    <t>256x256 with spatial bin 4. adc bin 1. all fit params free but shift fixed to 0</t>
-  </si>
-  <si>
     <t>chi sq (avg)</t>
   </si>
   <si>
     <t>average lifetime</t>
   </si>
   <si>
-    <t>binning</t>
-  </si>
-  <si>
     <t>fitting image</t>
   </si>
   <si>
-    <t>time elapsed (s)</t>
-  </si>
-  <si>
-    <t>rendering (1 overlay)</t>
-  </si>
-  <si>
     <t>&lt;- looking at tm only for ease right now</t>
   </si>
   <si>
@@ -97,14 +85,48 @@
   </si>
   <si>
     <t>probably still fine for a faster mode</t>
+  </si>
+  <si>
+    <t>2 exponential fit</t>
+  </si>
+  <si>
+    <t>2019-11-12 1-3 DMSO</t>
+  </si>
+  <si>
+    <t>other times:</t>
+  </si>
+  <si>
+    <t>binning a conc curve image: 0.27 sec</t>
+  </si>
+  <si>
+    <t>rendering (1 overlay): 2.5 sec</t>
+  </si>
+  <si>
+    <t>all fit params free, shift fixed to 0.</t>
+  </si>
+  <si>
+    <t>time (s)</t>
+  </si>
+  <si>
+    <t>all fits were standard spatial bin 4, adc bin 1 on 256x256</t>
+  </si>
+  <si>
+    <t>no downside here</t>
+  </si>
+  <si>
+    <t>seems ok too</t>
+  </si>
+  <si>
+    <t>recommendations for parameters</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -138,7 +160,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,6 +170,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -164,13 +192,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -178,6 +206,11 @@
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,51 +525,298 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC10102-7D9D-45CC-8D7B-C4FFE6CCE50F}">
-  <dimension ref="A14:O27"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="O30" sqref="O30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="9" max="9" width="12.77734375" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
-    <col min="12" max="12" width="15.44140625" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="14.88671875" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B5" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="G5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="N5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K6" t="s">
+        <v>9</v>
+      </c>
+      <c r="N6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1">
+        <v>100000</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="E7" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="G7" s="12">
+        <v>44.7</v>
+      </c>
+      <c r="I7">
+        <v>1.1597</v>
+      </c>
+      <c r="J7">
+        <v>1.5526</v>
+      </c>
+      <c r="K7">
+        <v>0.10730000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1">
+        <v>100000</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="E8" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="G8" s="12">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="I8">
+        <v>1.1600999999999999</v>
+      </c>
+      <c r="J8">
+        <v>1.5571999999999999</v>
+      </c>
+      <c r="K8">
+        <v>0.10680000000000001</v>
+      </c>
+      <c r="M8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1">
+        <v>100000</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="D9" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="G9" s="12">
+        <v>18.8</v>
+      </c>
+      <c r="I9">
+        <v>1.1785000000000001</v>
+      </c>
+      <c r="J9" s="9">
+        <v>1.6287</v>
+      </c>
+      <c r="K9">
+        <v>8.0299999999999996E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1">
+        <v>100000</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="E10" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="G10" s="12">
+        <v>30</v>
+      </c>
+      <c r="I10">
+        <v>1.1671</v>
+      </c>
+      <c r="J10" s="9">
+        <v>1.5717000000000001</v>
+      </c>
+      <c r="K10">
+        <v>0.1108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1">
+        <v>100000</v>
+      </c>
+      <c r="C11" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="E11" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="G11" s="12">
+        <v>42.4</v>
+      </c>
+      <c r="I11">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="J11">
+        <v>1.5529999999999999</v>
+      </c>
+      <c r="K11">
+        <v>0.10680000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="13">
+        <v>5</v>
+      </c>
+      <c r="B12" s="1">
+        <v>100000</v>
+      </c>
+      <c r="C12" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="G12" s="12">
+        <v>34</v>
+      </c>
+      <c r="I12">
+        <v>1.1603000000000001</v>
+      </c>
+      <c r="J12">
+        <v>1.5576000000000001</v>
+      </c>
+      <c r="K12">
+        <v>0.1071</v>
+      </c>
+      <c r="M12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B16" s="11" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B16" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="G16" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="K16" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="G16" s="6"/>
+      <c r="I16" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
         <v>0</v>
@@ -551,28 +831,22 @@
         <v>3</v>
       </c>
       <c r="G17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" t="s">
+        <v>4</v>
+      </c>
+      <c r="J17" t="s">
+        <v>5</v>
+      </c>
+      <c r="K17" t="s">
+        <v>9</v>
+      </c>
+      <c r="L17" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H17" t="s">
-        <v>8</v>
-      </c>
-      <c r="I17" t="s">
-        <v>10</v>
-      </c>
-      <c r="K17" t="s">
-        <v>5</v>
-      </c>
-      <c r="L17" t="s">
-        <v>6</v>
-      </c>
-      <c r="M17" t="s">
-        <v>13</v>
-      </c>
-      <c r="N17" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>0</v>
       </c>
@@ -589,25 +863,19 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="G18" s="2">
-        <v>0.26700000000000002</v>
-      </c>
-      <c r="H18" s="2">
         <v>88.5</v>
       </c>
-      <c r="I18" s="2">
-        <v>2.6</v>
+      <c r="I18" s="5">
+        <v>1.1288</v>
+      </c>
+      <c r="J18" s="5">
+        <v>0.27350000000000002</v>
       </c>
       <c r="K18" s="5">
-        <v>1.1288</v>
-      </c>
-      <c r="L18" s="5">
-        <v>0.27350000000000002</v>
-      </c>
-      <c r="M18" s="5">
         <v>3.3300000000000003E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1</v>
       </c>
@@ -623,23 +891,23 @@
       <c r="E19" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="H19">
+      <c r="G19">
         <v>79.3</v>
       </c>
+      <c r="I19">
+        <v>1.1324000000000001</v>
+      </c>
+      <c r="J19">
+        <v>0.2742</v>
+      </c>
       <c r="K19">
-        <v>1.1324000000000001</v>
-      </c>
-      <c r="L19">
-        <v>0.2742</v>
-      </c>
-      <c r="M19">
         <v>3.3500000000000002E-2</v>
       </c>
-      <c r="O19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2</v>
       </c>
@@ -655,23 +923,23 @@
       <c r="E20" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="H20">
+      <c r="G20">
         <v>56.7</v>
       </c>
+      <c r="I20">
+        <v>1.1591</v>
+      </c>
+      <c r="J20">
+        <v>0.28289999999999998</v>
+      </c>
       <c r="K20">
-        <v>1.1591</v>
-      </c>
-      <c r="L20">
-        <v>0.28289999999999998</v>
-      </c>
-      <c r="M20">
         <v>3.3799999999999997E-2</v>
       </c>
-      <c r="O20" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>3</v>
       </c>
@@ -687,20 +955,20 @@
       <c r="E21" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="H21">
+      <c r="G21">
         <v>48.2</v>
       </c>
-      <c r="K21" s="9">
+      <c r="I21" s="9">
         <v>1.3174999999999999</v>
       </c>
-      <c r="L21">
+      <c r="J21">
         <v>0.28010000000000002</v>
       </c>
-      <c r="M21">
+      <c r="K21">
         <v>3.5299999999999998E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>4</v>
       </c>
@@ -716,23 +984,23 @@
       <c r="E22" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="H22">
+      <c r="G22">
         <v>75.7</v>
       </c>
+      <c r="I22">
+        <v>1.1956</v>
+      </c>
+      <c r="J22">
+        <v>0.27439999999999998</v>
+      </c>
       <c r="K22">
-        <v>1.1956</v>
-      </c>
-      <c r="L22">
-        <v>0.27439999999999998</v>
-      </c>
-      <c r="M22">
-        <v>0.33</v>
-      </c>
-      <c r="O22" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="M22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>5</v>
       </c>
@@ -748,23 +1016,23 @@
       <c r="E23" s="8">
         <v>1E-4</v>
       </c>
-      <c r="H23">
+      <c r="G23">
         <v>86.7</v>
       </c>
+      <c r="I23">
+        <v>1.1288</v>
+      </c>
+      <c r="J23">
+        <v>0.27350000000000002</v>
+      </c>
       <c r="K23">
-        <v>1.1288</v>
-      </c>
-      <c r="L23">
-        <v>0.27350000000000002</v>
-      </c>
-      <c r="M23">
-        <v>0.33300000000000002</v>
-      </c>
-      <c r="O23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+        <v>3.3300000000000003E-2</v>
+      </c>
+      <c r="M23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>6</v>
       </c>
@@ -780,24 +1048,24 @@
       <c r="E24" s="8">
         <v>0.01</v>
       </c>
-      <c r="H24">
+      <c r="G24">
         <v>86.7</v>
       </c>
+      <c r="I24">
+        <v>1.1288</v>
+      </c>
+      <c r="J24">
+        <v>0.27350000000000002</v>
+      </c>
       <c r="K24">
-        <v>1.1288</v>
-      </c>
-      <c r="L24">
-        <v>0.27350000000000002</v>
-      </c>
-      <c r="M24">
-        <v>0.33300000000000002</v>
-      </c>
-      <c r="O24" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A25">
+        <v>3.3300000000000003E-2</v>
+      </c>
+      <c r="M24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="13">
         <v>7</v>
       </c>
       <c r="B25" s="1">
@@ -812,23 +1080,23 @@
       <c r="E25" s="8">
         <v>0.01</v>
       </c>
-      <c r="H25">
+      <c r="G25">
         <v>70</v>
       </c>
+      <c r="I25">
+        <v>1.1992</v>
+      </c>
+      <c r="J25">
+        <v>0.27479999999999999</v>
+      </c>
       <c r="K25">
-        <v>1.1992</v>
-      </c>
-      <c r="L25">
-        <v>0.27479999999999999</v>
-      </c>
-      <c r="M25">
-        <v>0.33300000000000002</v>
-      </c>
-      <c r="O25" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+        <v>3.3300000000000003E-2</v>
+      </c>
+      <c r="M25" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>8</v>
       </c>
@@ -844,23 +1112,23 @@
       <c r="E26" s="8">
         <v>0.01</v>
       </c>
-      <c r="H26">
+      <c r="G26">
         <v>48</v>
       </c>
+      <c r="I26">
+        <v>1.3174999999999999</v>
+      </c>
+      <c r="J26">
+        <v>0.28010000000000002</v>
+      </c>
       <c r="K26">
-        <v>1.3174999999999999</v>
-      </c>
-      <c r="L26">
-        <v>0.28010000000000002</v>
-      </c>
-      <c r="M26">
-        <v>0.35299999999999998</v>
-      </c>
-      <c r="O26" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+        <v>3.5299999999999998E-2</v>
+      </c>
+      <c r="M26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>9</v>
       </c>
@@ -876,27 +1144,28 @@
       <c r="E27" s="8">
         <v>0.01</v>
       </c>
-      <c r="H27">
+      <c r="G27">
         <v>45.2</v>
       </c>
+      <c r="I27">
+        <v>1.3289</v>
+      </c>
+      <c r="J27">
+        <v>0.2833</v>
+      </c>
       <c r="K27">
-        <v>1.3289</v>
-      </c>
-      <c r="L27">
-        <v>0.2833</v>
-      </c>
-      <c r="M27">
-        <v>0.35799999999999998</v>
-      </c>
-      <c r="O27" t="s">
-        <v>21</v>
+        <v>3.5799999999999998E-2</v>
+      </c>
+      <c r="M27" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B16:E16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="I5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>